<commit_message>
Fix color example to be wrapped by main function
</commit_message>
<xml_diff>
--- a/win32com/ex7_color.xlsx
+++ b/win32com/ex7_color.xlsx
@@ -16,6 +16,23 @@
     </ext>
   </extLst>
 </workbook>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+  <si>
+    <t>target</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>target</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>target</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -380,29 +397,40 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A6"/>
+  <dimension ref="A1:C6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C1" sqref="C1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="1"/>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="C1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="2"/>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" s="4"/>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="C3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" s="3"/>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" s="5"/>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" s="6"/>
+      <c r="C6" t="s">
+        <v>2</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>